<commit_message>
Added descriptions for cars
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyus\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\PHPClass\PHPGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B07C6FE7-43F9-4E87-B81F-CEAF41AAD9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2185EF91-3173-40BB-8CF4-E2FF3922018A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E8CBE3FD-DA7D-42A8-9739-0EAEF470F5E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E8CBE3FD-DA7D-42A8-9739-0EAEF470F5E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Make</t>
   </si>
@@ -135,6 +135,57 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>The Dodge Challenger (2017) is available for $37,590. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Ford F-150 XLT (2017) is available for $30,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Volkswagen Jetta Trendline (2023) is available for $23,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Honda Accord Touring 2.0 (2020) is available for $28,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Mazda CX-3 GX (2019) is available for $21,590. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Honda Civic Sedan Touring (2022) is available for $28,590. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Ford Mustang EcoBoost (2018) is available for $23,590. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Ford Mustang GT (2021) is available for $59,980. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Hyundai Ioniq 5 (2023) is available for $42,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Hyundai Elantra (2021) is available for $21,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Tesla Model 3 (2022) is available for $38,590. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Nissan Qashqai S (2021) is available for $19,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Hyundai Sonata Sport 1.6T (2022) is available for $24,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Kia Rio EX (2023) is available for $23,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Tesla Model 3 LR (2023) is available for $44,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Mazda Mazda 3 Sport GS (2024) is available for $28,990. It is a reliable choice offering a blend of performance and comfort.</t>
+  </si>
+  <si>
+    <t>The Ford Mustang V6 Coupe (2016) is available for $21,790. It is a reliable choice offering a blend of performance and comfort.</t>
   </si>
 </sst>
 </file>
@@ -509,7 +560,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +604,9 @@
       <c r="E2" t="s">
         <v>31</v>
       </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -570,6 +624,9 @@
       <c r="E3" t="s">
         <v>31</v>
       </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -587,6 +644,9 @@
       <c r="E4" t="s">
         <v>31</v>
       </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -604,6 +664,9 @@
       <c r="E5" t="s">
         <v>31</v>
       </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -621,6 +684,9 @@
       <c r="E6" t="s">
         <v>31</v>
       </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -638,6 +704,9 @@
       <c r="E7" t="s">
         <v>31</v>
       </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -655,6 +724,9 @@
       <c r="E8" t="s">
         <v>31</v>
       </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -672,6 +744,9 @@
       <c r="E9" t="s">
         <v>31</v>
       </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -689,6 +764,9 @@
       <c r="E10" t="s">
         <v>31</v>
       </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -706,6 +784,9 @@
       <c r="E11" t="s">
         <v>31</v>
       </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -723,6 +804,9 @@
       <c r="E12" t="s">
         <v>31</v>
       </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -740,6 +824,9 @@
       <c r="E13" t="s">
         <v>31</v>
       </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -757,6 +844,9 @@
       <c r="E14" t="s">
         <v>31</v>
       </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -774,6 +864,9 @@
       <c r="E15" t="s">
         <v>31</v>
       </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -791,8 +884,11 @@
       <c r="E16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -808,8 +904,11 @@
       <c r="E17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -824,6 +923,9 @@
       </c>
       <c r="E18" t="s">
         <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>